<commit_message>
Updated Process to open the websites with the data files
</commit_message>
<xml_diff>
--- a/UiPath/Diabetes_Risk_Assessor/Data/Input/DataSetPaths.xlsx
+++ b/UiPath/Diabetes_Risk_Assessor/Data/Input/DataSetPaths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/nlahanis_huronconsultinggroup_com/Documents/Documents/ML_RPA_Use_Cases/UiPath/Diabetes_Risk_Assessor/Data/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/aackerman_huronconsultinggroup_com/Documents/ML_RPA_Use_Cases/UiPath/Diabetes_Risk_Assessor/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{CB37CC12-6A50-493B-B89B-1B355532F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCAFE55E-2FC6-4C38-8D85-51EADD16F438}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{CB37CC12-6A50-493B-B89B-1B355532F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{223933F6-B8AF-4AC2-80CF-3B177DC1C576}"/>
   <bookViews>
-    <workbookView xWindow="-22785" yWindow="2745" windowWidth="16350" windowHeight="8955" xr2:uid="{486D5C5B-CE60-47FC-B352-3176255EB548}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{486D5C5B-CE60-47FC-B352-3176255EB548}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Paths" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>www.yahoo.com</t>
-  </si>
-  <si>
-    <t>www.google.com</t>
-  </si>
-  <si>
-    <t>www.apple.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Dataset Path</t>
   </si>
@@ -53,20 +44,47 @@
     <t>Dataset Name</t>
   </si>
   <si>
-    <t>Labs</t>
-  </si>
-  <si>
-    <t>Demographic</t>
-  </si>
-  <si>
-    <t>Blaha blaha</t>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Demographics&amp;CycleBeginYear=2017</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Dietary&amp;CycleBeginYear=2017</t>
+  </si>
+  <si>
+    <t>Dietary Data</t>
+  </si>
+  <si>
+    <t>Examination Data</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Examination&amp;CycleBeginYear=2017</t>
+  </si>
+  <si>
+    <t>Laboratory Data</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Laboratory&amp;CycleBeginYear=2017</t>
+  </si>
+  <si>
+    <t>Demographic Data</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Questionnaire&amp;CycleBeginYear=2017</t>
+  </si>
+  <si>
+    <t>Questionnaire Data</t>
+  </si>
+  <si>
+    <t>Limited Access Data</t>
+  </si>
+  <si>
+    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=LimitedAccess&amp;CycleBeginYear=2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +99,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212529"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,10 +127,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,10 +147,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -425,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD52F27-EB55-4249-9332-81496A26ABB7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,34 +460,58 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Process to download all XPT files
</commit_message>
<xml_diff>
--- a/UiPath/Diabetes_Risk_Assessor/Data/Input/DataSetPaths.xlsx
+++ b/UiPath/Diabetes_Risk_Assessor/Data/Input/DataSetPaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/aackerman_huronconsultinggroup_com/Documents/ML_RPA_Use_Cases/UiPath/Diabetes_Risk_Assessor/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="8_{CB37CC12-6A50-493B-B89B-1B355532F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{223933F6-B8AF-4AC2-80CF-3B177DC1C576}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{CB37CC12-6A50-493B-B89B-1B355532F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF99253F-1CD5-4278-9D74-A4BB38720E13}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{486D5C5B-CE60-47FC-B352-3176255EB548}"/>
+    <workbookView xWindow="-30828" yWindow="-8772" windowWidth="30936" windowHeight="16896" xr2:uid="{486D5C5B-CE60-47FC-B352-3176255EB548}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Paths" sheetId="1" r:id="rId1"/>
@@ -36,48 +36,276 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Dataset Path</t>
-  </si>
-  <si>
-    <t>Dataset Name</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Demographics&amp;CycleBeginYear=2017</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Dietary&amp;CycleBeginYear=2017</t>
-  </si>
-  <si>
-    <t>Dietary Data</t>
-  </si>
-  <si>
-    <t>Examination Data</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Examination&amp;CycleBeginYear=2017</t>
-  </si>
-  <si>
-    <t>Laboratory Data</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Laboratory&amp;CycleBeginYear=2017</t>
-  </si>
-  <si>
-    <t>Demographic Data</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=Questionnaire&amp;CycleBeginYear=2017</t>
-  </si>
-  <si>
-    <t>Questionnaire Data</t>
-  </si>
-  <si>
-    <t>Limited Access Data</t>
-  </si>
-  <si>
-    <t>https://wwwn.cdc.gov/nchs/nhanes/search/datapage.aspx?Component=LimitedAccess&amp;CycleBeginYear=2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+  <si>
+    <t>Acculturation</t>
+  </si>
+  <si>
+    <t>Alcohol Use</t>
+  </si>
+  <si>
+    <t>Audiometry</t>
+  </si>
+  <si>
+    <t>Blood Pressure &amp; Cholesterol</t>
+  </si>
+  <si>
+    <t>Cardiovascular Health</t>
+  </si>
+  <si>
+    <t>Consumer Behavior</t>
+  </si>
+  <si>
+    <t>Consumer Behavior Phone Follow-up Module - Adult</t>
+  </si>
+  <si>
+    <t>Consumer Behavior Phone Follow-up Module - Child</t>
+  </si>
+  <si>
+    <t>Current Health Status</t>
+  </si>
+  <si>
+    <t>Dermatology</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Diet Behavior &amp; Nutrition</t>
+  </si>
+  <si>
+    <t>Disability</t>
+  </si>
+  <si>
+    <t>Drug Use</t>
+  </si>
+  <si>
+    <t>Early Childhood</t>
+  </si>
+  <si>
+    <t>Food Security</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>Hepatitis</t>
+  </si>
+  <si>
+    <t>Hospital Utilization &amp; Access to Care</t>
+  </si>
+  <si>
+    <t>Housing Characteristics</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Kidney Conditions - Urology</t>
+  </si>
+  <si>
+    <t>Medical Conditions</t>
+  </si>
+  <si>
+    <t>Mental Health - Depression Screener</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Oral Health</t>
+  </si>
+  <si>
+    <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>Pesticide Use</t>
+  </si>
+  <si>
+    <t>Physical Activity</t>
+  </si>
+  <si>
+    <t>Physical Activity - Youth</t>
+  </si>
+  <si>
+    <t>Physical Functioning</t>
+  </si>
+  <si>
+    <t>Prescription Medications</t>
+  </si>
+  <si>
+    <t>Prescription Medications - Drug Information</t>
+  </si>
+  <si>
+    <t>Preventive Aspirin Use</t>
+  </si>
+  <si>
+    <t>Reproductive Health</t>
+  </si>
+  <si>
+    <t>Sleep Disorders</t>
+  </si>
+  <si>
+    <t>Smoking - Cigarette Use</t>
+  </si>
+  <si>
+    <t>Smoking - Household Smokers</t>
+  </si>
+  <si>
+    <t>Smoking - Recent Tobacco Use</t>
+  </si>
+  <si>
+    <t>Smoking - Secondhand Smoke Exposure</t>
+  </si>
+  <si>
+    <t>Volatile Toxicant</t>
+  </si>
+  <si>
+    <t>Weight History</t>
+  </si>
+  <si>
+    <t>Weight History - Youth</t>
+  </si>
+  <si>
+    <t>ACQ_J Data</t>
+  </si>
+  <si>
+    <t>ALQ_J Data</t>
+  </si>
+  <si>
+    <t>AUQ_J Data</t>
+  </si>
+  <si>
+    <t>BPQ_J Data</t>
+  </si>
+  <si>
+    <t>CDQ_J Data</t>
+  </si>
+  <si>
+    <t>CBQ_J Data</t>
+  </si>
+  <si>
+    <t>CBQPFA_J Data</t>
+  </si>
+  <si>
+    <t>CBQPFC_J Data</t>
+  </si>
+  <si>
+    <t>HSQ_J Data</t>
+  </si>
+  <si>
+    <t>DEQ_J Data</t>
+  </si>
+  <si>
+    <t>DIQ_J Data</t>
+  </si>
+  <si>
+    <t>DBQ_J Data</t>
+  </si>
+  <si>
+    <t>DLQ_J Data</t>
+  </si>
+  <si>
+    <t>DUQ_J Data</t>
+  </si>
+  <si>
+    <t>ECQ_J Data</t>
+  </si>
+  <si>
+    <t>FSQ_J Data</t>
+  </si>
+  <si>
+    <t>HIQ_J Data</t>
+  </si>
+  <si>
+    <t>HEQ_J Data</t>
+  </si>
+  <si>
+    <t>HUQ_J Data</t>
+  </si>
+  <si>
+    <t>HOQ_J Data</t>
+  </si>
+  <si>
+    <t>IMQ_J Data</t>
+  </si>
+  <si>
+    <t>INQ_J Data</t>
+  </si>
+  <si>
+    <t>KIQ_U_J Data</t>
+  </si>
+  <si>
+    <t>MCQ_J Data</t>
+  </si>
+  <si>
+    <t>DPQ_J Data</t>
+  </si>
+  <si>
+    <t>OCQ_J Data</t>
+  </si>
+  <si>
+    <t>OHQ_J Data</t>
+  </si>
+  <si>
+    <t>OSQ_J Data</t>
+  </si>
+  <si>
+    <t>PUQMEC_J Data</t>
+  </si>
+  <si>
+    <t>PAQ_J Data</t>
+  </si>
+  <si>
+    <t>PAQY_J Data</t>
+  </si>
+  <si>
+    <t>PFQ_J Data</t>
+  </si>
+  <si>
+    <t>RXQ_RX_J Data</t>
+  </si>
+  <si>
+    <t>RXQ_DRUG Data</t>
+  </si>
+  <si>
+    <t>RXQASA_J Data</t>
+  </si>
+  <si>
+    <t>RHQ_J Data</t>
+  </si>
+  <si>
+    <t>SLQ_J Data</t>
+  </si>
+  <si>
+    <t>SMQ_J Data</t>
+  </si>
+  <si>
+    <t>SMQFAM_J Data</t>
+  </si>
+  <si>
+    <t>SMQRTU_J Data</t>
+  </si>
+  <si>
+    <t>SMQSHS_J Data</t>
+  </si>
+  <si>
+    <t>VTQ_J Data</t>
+  </si>
+  <si>
+    <t>WHQ_J Data</t>
+  </si>
+  <si>
+    <t>WHQMEC_J Data</t>
+  </si>
+  <si>
+    <t>Data File</t>
+  </si>
+  <si>
+    <t>Data File Name</t>
   </si>
 </sst>
 </file>
@@ -93,18 +321,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF212529"/>
-      <name val="Open Sans"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,10 +356,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -147,6 +375,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,72 +678,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD52F27-EB55-4249-9332-81496A26ABB7}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
+      <c r="B15" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>